<commit_message>
index update for Political Data
</commit_message>
<xml_diff>
--- a/slides/courses/analysisOfPoliticalData/schedule_editable.xlsx
+++ b/slides/courses/analysisOfPoliticalData/schedule_editable.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10907"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Seafile\WW\03_Employment\01_Teaching\01_courses\01_Analysis_of_Political_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCCE7E1-5206-4D0C-B620-AE75006B0236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24F47E5E-03D6-B148-B5CC-B65916144CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="0" windowWidth="25980" windowHeight="16200" xr2:uid="{78EE7E86-4C0C-459A-920A-BF97E70E6E2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>topic</t>
   </si>
@@ -225,9 +227,6 @@
     <t>关联性统计</t>
   </si>
   <si>
-    <t>循环与批处理</t>
-  </si>
-  <si>
     <t>基础可视化</t>
   </si>
   <si>
@@ -291,10 +290,28 @@
     <t>Regular expression</t>
   </si>
   <si>
-    <t>@King1995;@WonnacottWonnacott1978[chap. 2]; @MooreSiegel2013[chap. 9]; @ChenZhengChangJiaJunPing2016[chap. 1].</t>
-  </si>
-  <si>
     <t>@Wooldridge2016[chap. 4, 6].</t>
+  </si>
+  <si>
+    <t>Course Introduction</t>
+  </si>
+  <si>
+    <t>课程介绍</t>
+  </si>
+  <si>
+    <t>@WonnacottWonnacott1978[chap. 2]; @MooreSiegel2013[chap. 9]; @ChenZhengChangJiaJunPing2016[chap. 1].</t>
+  </si>
+  <si>
+    <t>@King1995</t>
+  </si>
+  <si>
+    <t>批处理</t>
+  </si>
+  <si>
+    <t>循环</t>
+  </si>
+  <si>
+    <t>Batching</t>
   </si>
 </sst>
 </file>
@@ -338,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -354,7 +371,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,23 +667,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EBEFF0-276E-440A-92F1-EDEAEA941110}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="106.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.10546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.67578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.0546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -683,18 +700,18 @@
         <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>58</v>
@@ -703,15 +720,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
@@ -720,15 +737,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -737,15 +754,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -754,15 +771,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -771,15 +788,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>62</v>
@@ -788,181 +805,198 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>64</v>
       </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
         <v>69</v>
       </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>52</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>